<commit_message>
Update columns configuration, drop time filter to 120 seconds if top 100 AWC is selected.
</commit_message>
<xml_diff>
--- a/output/SAMPLE_INPUT_100snippets_awc.xlsx
+++ b/output/SAMPLE_INPUT_100snippets_awc.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G101"/>
+  <dimension ref="A1:F101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,30 +441,25 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Time</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
           <t>SegStart</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>SegEnd</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>AWC</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>TVN</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>CTC</t>
         </is>
@@ -474,24 +469,19 @@
       <c r="A2" t="n">
         <v>1</v>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>5:25 AM</t>
-        </is>
+      <c r="B2" t="n">
+        <v>8.733333</v>
       </c>
       <c r="C2" t="n">
-        <v>8.733333</v>
+        <v>38.733333</v>
       </c>
       <c r="D2" t="n">
-        <v>38.733333</v>
+        <v>12.843333</v>
       </c>
       <c r="E2" t="n">
-        <v>12.843333</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -499,24 +489,19 @@
       <c r="A3" t="n">
         <v>10</v>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>5:30 AM</t>
-        </is>
+      <c r="B3" t="n">
+        <v>282.885</v>
       </c>
       <c r="C3" t="n">
-        <v>282.885</v>
+        <v>312.885</v>
       </c>
       <c r="D3" t="n">
-        <v>312.885</v>
+        <v>14.155</v>
       </c>
       <c r="E3" t="n">
-        <v>14.155</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -524,24 +509,19 @@
       <c r="A4" t="n">
         <v>25</v>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>5:37 AM</t>
-        </is>
+      <c r="B4" t="n">
+        <v>729.045</v>
       </c>
       <c r="C4" t="n">
-        <v>729.045</v>
+        <v>759.045</v>
       </c>
       <c r="D4" t="n">
-        <v>759.045</v>
+        <v>11.335</v>
       </c>
       <c r="E4" t="n">
-        <v>11.335</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -549,24 +529,19 @@
       <c r="A5" t="n">
         <v>39</v>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>5:45 AM</t>
-        </is>
+      <c r="B5" t="n">
+        <v>1169.48</v>
       </c>
       <c r="C5" t="n">
-        <v>1169.48</v>
+        <v>1199.48</v>
       </c>
       <c r="D5" t="n">
-        <v>1199.48</v>
+        <v>21.87</v>
       </c>
       <c r="E5" t="n">
-        <v>21.87</v>
+        <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" t="n">
         <v>2</v>
       </c>
     </row>
@@ -574,24 +549,19 @@
       <c r="A6" t="n">
         <v>49</v>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>5:50 AM</t>
-        </is>
+      <c r="B6" t="n">
+        <v>1467.18</v>
       </c>
       <c r="C6" t="n">
-        <v>1467.18</v>
+        <v>1497.18</v>
       </c>
       <c r="D6" t="n">
-        <v>1497.18</v>
+        <v>24.93</v>
       </c>
       <c r="E6" t="n">
-        <v>24.93</v>
+        <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" t="n">
         <v>1</v>
       </c>
     </row>
@@ -599,24 +569,19 @@
       <c r="A7" t="n">
         <v>61</v>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>5:55 AM</t>
-        </is>
+      <c r="B7" t="n">
+        <v>1813.59</v>
       </c>
       <c r="C7" t="n">
-        <v>1813.59</v>
+        <v>1843.59</v>
       </c>
       <c r="D7" t="n">
-        <v>1843.59</v>
+        <v>7.55</v>
       </c>
       <c r="E7" t="n">
-        <v>7.55</v>
+        <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
-      </c>
-      <c r="G7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -624,24 +589,19 @@
       <c r="A8" t="n">
         <v>71</v>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>6:00 AM</t>
-        </is>
+      <c r="B8" t="n">
+        <v>2110.065</v>
       </c>
       <c r="C8" t="n">
-        <v>2110.065</v>
+        <v>2140.065</v>
       </c>
       <c r="D8" t="n">
-        <v>2140.065</v>
+        <v>8.81</v>
       </c>
       <c r="E8" t="n">
-        <v>8.81</v>
+        <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>0</v>
-      </c>
-      <c r="G8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -649,24 +609,19 @@
       <c r="A9" t="n">
         <v>78</v>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>6:04 AM</t>
-        </is>
+      <c r="B9" t="n">
+        <v>2326.65</v>
       </c>
       <c r="C9" t="n">
-        <v>2326.65</v>
+        <v>2356.65</v>
       </c>
       <c r="D9" t="n">
-        <v>2356.65</v>
+        <v>14.63</v>
       </c>
       <c r="E9" t="n">
-        <v>14.63</v>
+        <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>0</v>
-      </c>
-      <c r="G9" t="n">
         <v>0</v>
       </c>
     </row>
@@ -674,24 +629,19 @@
       <c r="A10" t="n">
         <v>91</v>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>6:11 AM</t>
-        </is>
+      <c r="B10" t="n">
+        <v>2725.88</v>
       </c>
       <c r="C10" t="n">
-        <v>2725.88</v>
+        <v>2755.88</v>
       </c>
       <c r="D10" t="n">
-        <v>2755.88</v>
+        <v>22.16</v>
       </c>
       <c r="E10" t="n">
-        <v>22.16</v>
+        <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>0</v>
-      </c>
-      <c r="G10" t="n">
         <v>0</v>
       </c>
     </row>
@@ -699,24 +649,19 @@
       <c r="A11" t="n">
         <v>100</v>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>6:15 AM</t>
-        </is>
+      <c r="B11" t="n">
+        <v>2986.3175</v>
       </c>
       <c r="C11" t="n">
-        <v>2986.3175</v>
+        <v>3016.3175</v>
       </c>
       <c r="D11" t="n">
-        <v>3016.3175</v>
+        <v>30.9975</v>
       </c>
       <c r="E11" t="n">
-        <v>30.9975</v>
+        <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>0</v>
-      </c>
-      <c r="G11" t="n">
         <v>1.25</v>
       </c>
     </row>
@@ -724,24 +669,19 @@
       <c r="A12" t="n">
         <v>108</v>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>6:19 AM</t>
-        </is>
+      <c r="B12" t="n">
+        <v>3217.113333</v>
       </c>
       <c r="C12" t="n">
-        <v>3217.113333</v>
+        <v>3247.113333</v>
       </c>
       <c r="D12" t="n">
-        <v>3247.113333</v>
+        <v>16.883333</v>
       </c>
       <c r="E12" t="n">
-        <v>16.883333</v>
+        <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>0</v>
-      </c>
-      <c r="G12" t="n">
         <v>1.333333</v>
       </c>
     </row>
@@ -749,24 +689,19 @@
       <c r="A13" t="n">
         <v>120</v>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>6:25 AM</t>
-        </is>
+      <c r="B13" t="n">
+        <v>3577.16</v>
       </c>
       <c r="C13" t="n">
-        <v>3577.16</v>
+        <v>3607.16</v>
       </c>
       <c r="D13" t="n">
-        <v>3607.16</v>
+        <v>49.37</v>
       </c>
       <c r="E13" t="n">
-        <v>49.37</v>
+        <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>0</v>
-      </c>
-      <c r="G13" t="n">
         <v>0</v>
       </c>
     </row>
@@ -774,24 +709,19 @@
       <c r="A14" t="n">
         <v>136</v>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>6:33 AM</t>
-        </is>
+      <c r="B14" t="n">
+        <v>4068.95</v>
       </c>
       <c r="C14" t="n">
-        <v>4068.95</v>
+        <v>4098.95</v>
       </c>
       <c r="D14" t="n">
-        <v>4098.95</v>
+        <v>5.37</v>
       </c>
       <c r="E14" t="n">
-        <v>5.37</v>
+        <v>0</v>
       </c>
       <c r="F14" t="n">
-        <v>0</v>
-      </c>
-      <c r="G14" t="n">
         <v>0.333333</v>
       </c>
     </row>
@@ -799,24 +729,19 @@
       <c r="A15" t="n">
         <v>143</v>
       </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>6:36 AM</t>
-        </is>
+      <c r="B15" t="n">
+        <v>4280.55</v>
       </c>
       <c r="C15" t="n">
-        <v>4280.55</v>
+        <v>4310.55</v>
       </c>
       <c r="D15" t="n">
-        <v>4310.55</v>
+        <v>3.255</v>
       </c>
       <c r="E15" t="n">
-        <v>3.255</v>
+        <v>0</v>
       </c>
       <c r="F15" t="n">
-        <v>0</v>
-      </c>
-      <c r="G15" t="n">
         <v>0</v>
       </c>
     </row>
@@ -824,24 +749,19 @@
       <c r="A16" t="n">
         <v>151</v>
       </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>6:40 AM</t>
-        </is>
+      <c r="B16" t="n">
+        <v>4506.15</v>
       </c>
       <c r="C16" t="n">
-        <v>4506.15</v>
+        <v>4536.15</v>
       </c>
       <c r="D16" t="n">
-        <v>4536.15</v>
+        <v>33.81</v>
       </c>
       <c r="E16" t="n">
-        <v>33.81</v>
+        <v>0</v>
       </c>
       <c r="F16" t="n">
-        <v>0</v>
-      </c>
-      <c r="G16" t="n">
         <v>1</v>
       </c>
     </row>
@@ -849,24 +769,19 @@
       <c r="A17" t="n">
         <v>160</v>
       </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>6:45 AM</t>
-        </is>
+      <c r="B17" t="n">
+        <v>4780.59</v>
       </c>
       <c r="C17" t="n">
-        <v>4780.59</v>
+        <v>4810.59</v>
       </c>
       <c r="D17" t="n">
-        <v>4810.59</v>
+        <v>5.99</v>
       </c>
       <c r="E17" t="n">
-        <v>5.99</v>
+        <v>0</v>
       </c>
       <c r="F17" t="n">
-        <v>0</v>
-      </c>
-      <c r="G17" t="n">
         <v>0</v>
       </c>
     </row>
@@ -874,24 +789,19 @@
       <c r="A18" t="n">
         <v>174</v>
       </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>6:52 AM</t>
-        </is>
+      <c r="B18" t="n">
+        <v>5193.04</v>
       </c>
       <c r="C18" t="n">
-        <v>5193.04</v>
+        <v>5223.04</v>
       </c>
       <c r="D18" t="n">
-        <v>5223.04</v>
+        <v>71.97</v>
       </c>
       <c r="E18" t="n">
-        <v>71.97</v>
+        <v>0</v>
       </c>
       <c r="F18" t="n">
-        <v>0</v>
-      </c>
-      <c r="G18" t="n">
         <v>0</v>
       </c>
     </row>
@@ -899,24 +809,19 @@
       <c r="A19" t="n">
         <v>182</v>
       </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>6:56 AM</t>
-        </is>
+      <c r="B19" t="n">
+        <v>5440.89</v>
       </c>
       <c r="C19" t="n">
-        <v>5440.89</v>
+        <v>5470.89</v>
       </c>
       <c r="D19" t="n">
-        <v>5470.89</v>
+        <v>108.74</v>
       </c>
       <c r="E19" t="n">
-        <v>108.74</v>
+        <v>0</v>
       </c>
       <c r="F19" t="n">
-        <v>0</v>
-      </c>
-      <c r="G19" t="n">
         <v>0</v>
       </c>
     </row>
@@ -924,24 +829,19 @@
       <c r="A20" t="n">
         <v>193</v>
       </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>7:01 AM</t>
-        </is>
+      <c r="B20" t="n">
+        <v>5776.925</v>
       </c>
       <c r="C20" t="n">
-        <v>5776.925</v>
+        <v>5806.925</v>
       </c>
       <c r="D20" t="n">
-        <v>5806.925</v>
+        <v>13.53</v>
       </c>
       <c r="E20" t="n">
-        <v>13.53</v>
+        <v>0</v>
       </c>
       <c r="F20" t="n">
-        <v>0</v>
-      </c>
-      <c r="G20" t="n">
         <v>0</v>
       </c>
     </row>
@@ -949,24 +849,19 @@
       <c r="A21" t="n">
         <v>204</v>
       </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>7:07 AM</t>
-        </is>
+      <c r="B21" t="n">
+        <v>6102.224</v>
       </c>
       <c r="C21" t="n">
-        <v>6102.224</v>
+        <v>6132.224</v>
       </c>
       <c r="D21" t="n">
-        <v>6132.224</v>
+        <v>3.75</v>
       </c>
       <c r="E21" t="n">
-        <v>3.75</v>
+        <v>0</v>
       </c>
       <c r="F21" t="n">
-        <v>0</v>
-      </c>
-      <c r="G21" t="n">
         <v>0</v>
       </c>
     </row>
@@ -974,24 +869,19 @@
       <c r="A22" t="n">
         <v>220</v>
       </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>7:15 AM</t>
-        </is>
+      <c r="B22" t="n">
+        <v>6584.895</v>
       </c>
       <c r="C22" t="n">
-        <v>6584.895</v>
+        <v>6614.895</v>
       </c>
       <c r="D22" t="n">
-        <v>6614.895</v>
+        <v>9.41</v>
       </c>
       <c r="E22" t="n">
-        <v>9.41</v>
+        <v>0</v>
       </c>
       <c r="F22" t="n">
-        <v>0</v>
-      </c>
-      <c r="G22" t="n">
         <v>0</v>
       </c>
     </row>
@@ -999,24 +889,19 @@
       <c r="A23" t="n">
         <v>230</v>
       </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>7:20 AM</t>
-        </is>
+      <c r="B23" t="n">
+        <v>6880.786667</v>
       </c>
       <c r="C23" t="n">
-        <v>6880.786667</v>
+        <v>6910.786667</v>
       </c>
       <c r="D23" t="n">
-        <v>6910.786667</v>
+        <v>32.193333</v>
       </c>
       <c r="E23" t="n">
-        <v>32.193333</v>
+        <v>0</v>
       </c>
       <c r="F23" t="n">
-        <v>0</v>
-      </c>
-      <c r="G23" t="n">
         <v>1.333333</v>
       </c>
     </row>
@@ -1024,24 +909,19 @@
       <c r="A24" t="n">
         <v>239</v>
       </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>7:24 AM</t>
-        </is>
+      <c r="B24" t="n">
+        <v>7146.62</v>
       </c>
       <c r="C24" t="n">
-        <v>7146.62</v>
+        <v>7176.62</v>
       </c>
       <c r="D24" t="n">
-        <v>7176.62</v>
+        <v>32.95</v>
       </c>
       <c r="E24" t="n">
-        <v>32.95</v>
+        <v>0</v>
       </c>
       <c r="F24" t="n">
-        <v>0</v>
-      </c>
-      <c r="G24" t="n">
         <v>2</v>
       </c>
     </row>
@@ -1049,24 +929,19 @@
       <c r="A25" t="n">
         <v>249</v>
       </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>7:29 AM</t>
-        </is>
+      <c r="B25" t="n">
+        <v>7455.21</v>
       </c>
       <c r="C25" t="n">
-        <v>7455.21</v>
+        <v>7485.21</v>
       </c>
       <c r="D25" t="n">
-        <v>7485.21</v>
+        <v>11.435</v>
       </c>
       <c r="E25" t="n">
-        <v>11.435</v>
+        <v>0</v>
       </c>
       <c r="F25" t="n">
-        <v>0</v>
-      </c>
-      <c r="G25" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1074,24 +949,19 @@
       <c r="A26" t="n">
         <v>257</v>
       </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>7:33 AM</t>
-        </is>
+      <c r="B26" t="n">
+        <v>7691.65</v>
       </c>
       <c r="C26" t="n">
-        <v>7691.65</v>
+        <v>7721.65</v>
       </c>
       <c r="D26" t="n">
-        <v>7721.65</v>
+        <v>35.775</v>
       </c>
       <c r="E26" t="n">
-        <v>35.775</v>
+        <v>0</v>
       </c>
       <c r="F26" t="n">
-        <v>0</v>
-      </c>
-      <c r="G26" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1099,24 +969,19 @@
       <c r="A27" t="n">
         <v>275</v>
       </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>7:43 AM</t>
-        </is>
+      <c r="B27" t="n">
+        <v>8248.530000000001</v>
       </c>
       <c r="C27" t="n">
-        <v>8248.530000000001</v>
+        <v>8278.530000000001</v>
       </c>
       <c r="D27" t="n">
-        <v>8278.530000000001</v>
+        <v>21.35</v>
       </c>
       <c r="E27" t="n">
-        <v>21.35</v>
+        <v>0</v>
       </c>
       <c r="F27" t="n">
-        <v>0</v>
-      </c>
-      <c r="G27" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1124,24 +989,19 @@
       <c r="A28" t="n">
         <v>286</v>
       </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>7:48 AM</t>
-        </is>
+      <c r="B28" t="n">
+        <v>8565.615</v>
       </c>
       <c r="C28" t="n">
-        <v>8565.615</v>
+        <v>8595.615</v>
       </c>
       <c r="D28" t="n">
-        <v>8595.615</v>
+        <v>3.93</v>
       </c>
       <c r="E28" t="n">
-        <v>3.93</v>
+        <v>0</v>
       </c>
       <c r="F28" t="n">
-        <v>0</v>
-      </c>
-      <c r="G28" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1149,24 +1009,19 @@
       <c r="A29" t="n">
         <v>293</v>
       </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>7:51 AM</t>
-        </is>
+      <c r="B29" t="n">
+        <v>8779.4</v>
       </c>
       <c r="C29" t="n">
-        <v>8779.4</v>
+        <v>8809.4</v>
       </c>
       <c r="D29" t="n">
-        <v>8809.4</v>
+        <v>11.2</v>
       </c>
       <c r="E29" t="n">
-        <v>11.2</v>
+        <v>0</v>
       </c>
       <c r="F29" t="n">
-        <v>0</v>
-      </c>
-      <c r="G29" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1174,24 +1029,19 @@
       <c r="A30" t="n">
         <v>307</v>
       </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>7:58 AM</t>
-        </is>
+      <c r="B30" t="n">
+        <v>9193.143333</v>
       </c>
       <c r="C30" t="n">
-        <v>9193.143333</v>
+        <v>9223.143333</v>
       </c>
       <c r="D30" t="n">
-        <v>9223.143333</v>
+        <v>12.653333</v>
       </c>
       <c r="E30" t="n">
-        <v>12.653333</v>
+        <v>0</v>
       </c>
       <c r="F30" t="n">
-        <v>0</v>
-      </c>
-      <c r="G30" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1199,24 +1049,19 @@
       <c r="A31" t="n">
         <v>321</v>
       </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>8:05 AM</t>
-        </is>
+      <c r="B31" t="n">
+        <v>9601.75</v>
       </c>
       <c r="C31" t="n">
-        <v>9601.75</v>
+        <v>9631.75</v>
       </c>
       <c r="D31" t="n">
-        <v>9631.75</v>
+        <v>3.92</v>
       </c>
       <c r="E31" t="n">
-        <v>3.92</v>
+        <v>0</v>
       </c>
       <c r="F31" t="n">
-        <v>0</v>
-      </c>
-      <c r="G31" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1224,24 +1069,19 @@
       <c r="A32" t="n">
         <v>331</v>
       </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>8:10 AM</t>
-        </is>
+      <c r="B32" t="n">
+        <v>9903.9</v>
       </c>
       <c r="C32" t="n">
-        <v>9903.9</v>
+        <v>9933.9</v>
       </c>
       <c r="D32" t="n">
-        <v>9933.9</v>
+        <v>66.37</v>
       </c>
       <c r="E32" t="n">
-        <v>66.37</v>
+        <v>0</v>
       </c>
       <c r="F32" t="n">
-        <v>0</v>
-      </c>
-      <c r="G32" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1249,24 +1089,19 @@
       <c r="A33" t="n">
         <v>339</v>
       </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>8:14 AM</t>
-        </is>
+      <c r="B33" t="n">
+        <v>10144.22</v>
       </c>
       <c r="C33" t="n">
-        <v>10144.22</v>
+        <v>10174.22</v>
       </c>
       <c r="D33" t="n">
-        <v>10174.22</v>
+        <v>2.585</v>
       </c>
       <c r="E33" t="n">
-        <v>2.585</v>
+        <v>0</v>
       </c>
       <c r="F33" t="n">
-        <v>0</v>
-      </c>
-      <c r="G33" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1274,24 +1109,19 @@
       <c r="A34" t="n">
         <v>350</v>
       </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>8:20 AM</t>
-        </is>
+      <c r="B34" t="n">
+        <v>10490.436667</v>
       </c>
       <c r="C34" t="n">
-        <v>10490.436667</v>
+        <v>10520.436667</v>
       </c>
       <c r="D34" t="n">
-        <v>10520.436667</v>
+        <v>4.836667</v>
       </c>
       <c r="E34" t="n">
-        <v>4.836667</v>
+        <v>0</v>
       </c>
       <c r="F34" t="n">
-        <v>0</v>
-      </c>
-      <c r="G34" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1299,24 +1129,19 @@
       <c r="A35" t="n">
         <v>365</v>
       </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>8:27 AM</t>
-        </is>
+      <c r="B35" t="n">
+        <v>10930.83</v>
       </c>
       <c r="C35" t="n">
-        <v>10930.83</v>
+        <v>10960.83</v>
       </c>
       <c r="D35" t="n">
-        <v>10960.83</v>
+        <v>15.57</v>
       </c>
       <c r="E35" t="n">
-        <v>15.57</v>
+        <v>0</v>
       </c>
       <c r="F35" t="n">
-        <v>0</v>
-      </c>
-      <c r="G35" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1324,24 +1149,19 @@
       <c r="A36" t="n">
         <v>378</v>
       </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>8:34 AM</t>
-        </is>
+      <c r="B36" t="n">
+        <v>11323.225</v>
       </c>
       <c r="C36" t="n">
-        <v>11323.225</v>
+        <v>11353.225</v>
       </c>
       <c r="D36" t="n">
-        <v>11353.225</v>
+        <v>8.6</v>
       </c>
       <c r="E36" t="n">
-        <v>8.6</v>
+        <v>0</v>
       </c>
       <c r="F36" t="n">
-        <v>0</v>
-      </c>
-      <c r="G36" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1349,24 +1169,19 @@
       <c r="A37" t="n">
         <v>387</v>
       </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>8:39 AM</t>
-        </is>
+      <c r="B37" t="n">
+        <v>11609.42</v>
       </c>
       <c r="C37" t="n">
-        <v>11609.42</v>
+        <v>11639.42</v>
       </c>
       <c r="D37" t="n">
-        <v>11639.42</v>
+        <v>8.06</v>
       </c>
       <c r="E37" t="n">
-        <v>8.06</v>
+        <v>0</v>
       </c>
       <c r="F37" t="n">
-        <v>0</v>
-      </c>
-      <c r="G37" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1374,24 +1189,19 @@
       <c r="A38" t="n">
         <v>425</v>
       </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>8:57 AM</t>
-        </is>
+      <c r="B38" t="n">
+        <v>12725.265</v>
       </c>
       <c r="C38" t="n">
-        <v>12725.265</v>
+        <v>12755.265</v>
       </c>
       <c r="D38" t="n">
-        <v>12755.265</v>
+        <v>4.76</v>
       </c>
       <c r="E38" t="n">
-        <v>4.76</v>
+        <v>43.895</v>
       </c>
       <c r="F38" t="n">
-        <v>43.895</v>
-      </c>
-      <c r="G38" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1399,24 +1209,19 @@
       <c r="A39" t="n">
         <v>435</v>
       </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>9:02 AM</t>
-        </is>
+      <c r="B39" t="n">
+        <v>13043.06</v>
       </c>
       <c r="C39" t="n">
-        <v>13043.06</v>
+        <v>13073.06</v>
       </c>
       <c r="D39" t="n">
-        <v>13073.06</v>
+        <v>4.12</v>
       </c>
       <c r="E39" t="n">
-        <v>4.12</v>
+        <v>1.68</v>
       </c>
       <c r="F39" t="n">
-        <v>1.68</v>
-      </c>
-      <c r="G39" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1424,24 +1229,19 @@
       <c r="A40" t="n">
         <v>451</v>
       </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>9:10 AM</t>
-        </is>
+      <c r="B40" t="n">
+        <v>13511.86</v>
       </c>
       <c r="C40" t="n">
-        <v>13511.86</v>
+        <v>13541.86</v>
       </c>
       <c r="D40" t="n">
-        <v>13541.86</v>
+        <v>5.205</v>
       </c>
       <c r="E40" t="n">
-        <v>5.205</v>
+        <v>10.74</v>
       </c>
       <c r="F40" t="n">
-        <v>10.74</v>
-      </c>
-      <c r="G40" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -1449,24 +1249,19 @@
       <c r="A41" t="n">
         <v>472</v>
       </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>9:21 AM</t>
-        </is>
+      <c r="B41" t="n">
+        <v>14149.596667</v>
       </c>
       <c r="C41" t="n">
-        <v>14149.596667</v>
+        <v>14179.596667</v>
       </c>
       <c r="D41" t="n">
-        <v>14179.596667</v>
+        <v>5.256667</v>
       </c>
       <c r="E41" t="n">
-        <v>5.256667</v>
+        <v>5.23</v>
       </c>
       <c r="F41" t="n">
-        <v>5.23</v>
-      </c>
-      <c r="G41" t="n">
         <v>0.333333</v>
       </c>
     </row>
@@ -1474,24 +1269,19 @@
       <c r="A42" t="n">
         <v>482</v>
       </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>9:26 AM</t>
-        </is>
+      <c r="B42" t="n">
+        <v>14442.785</v>
       </c>
       <c r="C42" t="n">
-        <v>14442.785</v>
+        <v>14472.785</v>
       </c>
       <c r="D42" t="n">
-        <v>14472.785</v>
+        <v>8.75</v>
       </c>
       <c r="E42" t="n">
-        <v>8.75</v>
+        <v>7.99</v>
       </c>
       <c r="F42" t="n">
-        <v>7.99</v>
-      </c>
-      <c r="G42" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1499,24 +1289,19 @@
       <c r="A43" t="n">
         <v>502</v>
       </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>9:36 AM</t>
-        </is>
+      <c r="B43" t="n">
+        <v>15056.18</v>
       </c>
       <c r="C43" t="n">
-        <v>15056.18</v>
+        <v>15086.18</v>
       </c>
       <c r="D43" t="n">
-        <v>15086.18</v>
+        <v>6.085</v>
       </c>
       <c r="E43" t="n">
-        <v>6.085</v>
+        <v>24.46</v>
       </c>
       <c r="F43" t="n">
-        <v>24.46</v>
-      </c>
-      <c r="G43" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -1524,24 +1309,19 @@
       <c r="A44" t="n">
         <v>512</v>
       </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>9:41 AM</t>
-        </is>
+      <c r="B44" t="n">
+        <v>15345.09</v>
       </c>
       <c r="C44" t="n">
-        <v>15345.09</v>
+        <v>15375.09</v>
       </c>
       <c r="D44" t="n">
-        <v>15375.09</v>
+        <v>3.238333</v>
       </c>
       <c r="E44" t="n">
-        <v>3.238333</v>
+        <v>2.291667</v>
       </c>
       <c r="F44" t="n">
-        <v>2.291667</v>
-      </c>
-      <c r="G44" t="n">
         <v>0.166667</v>
       </c>
     </row>
@@ -1549,24 +1329,19 @@
       <c r="A45" t="n">
         <v>524</v>
       </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>9:47 AM</t>
-        </is>
+      <c r="B45" t="n">
+        <v>15702.116667</v>
       </c>
       <c r="C45" t="n">
-        <v>15702.116667</v>
+        <v>15732.116667</v>
       </c>
       <c r="D45" t="n">
-        <v>15732.116667</v>
+        <v>35.09</v>
       </c>
       <c r="E45" t="n">
-        <v>35.09</v>
+        <v>0</v>
       </c>
       <c r="F45" t="n">
-        <v>0</v>
-      </c>
-      <c r="G45" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1574,24 +1349,19 @@
       <c r="A46" t="n">
         <v>550</v>
       </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>10:00 A</t>
-        </is>
+      <c r="B46" t="n">
+        <v>16484</v>
       </c>
       <c r="C46" t="n">
-        <v>16484</v>
+        <v>16514</v>
       </c>
       <c r="D46" t="n">
-        <v>16514</v>
+        <v>26.08</v>
       </c>
       <c r="E46" t="n">
-        <v>26.08</v>
+        <v>0</v>
       </c>
       <c r="F46" t="n">
-        <v>0</v>
-      </c>
-      <c r="G46" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1599,24 +1369,19 @@
       <c r="A47" t="n">
         <v>570</v>
       </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>10:10 A</t>
-        </is>
+      <c r="B47" t="n">
+        <v>17087.03</v>
       </c>
       <c r="C47" t="n">
-        <v>17087.03</v>
+        <v>17117.03</v>
       </c>
       <c r="D47" t="n">
-        <v>17117.03</v>
+        <v>37.05</v>
       </c>
       <c r="E47" t="n">
-        <v>37.05</v>
+        <v>0</v>
       </c>
       <c r="F47" t="n">
-        <v>0</v>
-      </c>
-      <c r="G47" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1624,24 +1389,19 @@
       <c r="A48" t="n">
         <v>578</v>
       </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>10:14 A</t>
-        </is>
+      <c r="B48" t="n">
+        <v>17339.01</v>
       </c>
       <c r="C48" t="n">
-        <v>17339.01</v>
+        <v>17369.01</v>
       </c>
       <c r="D48" t="n">
-        <v>17369.01</v>
+        <v>5.25</v>
       </c>
       <c r="E48" t="n">
-        <v>5.25</v>
+        <v>0</v>
       </c>
       <c r="F48" t="n">
-        <v>0</v>
-      </c>
-      <c r="G48" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1649,24 +1409,19 @@
       <c r="A49" t="n">
         <v>981</v>
       </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>1:35 PM</t>
-        </is>
+      <c r="B49" t="n">
+        <v>29415.15</v>
       </c>
       <c r="C49" t="n">
-        <v>29415.15</v>
+        <v>29445.15</v>
       </c>
       <c r="D49" t="n">
-        <v>29445.15</v>
+        <v>13.746667</v>
       </c>
       <c r="E49" t="n">
-        <v>13.746667</v>
+        <v>0</v>
       </c>
       <c r="F49" t="n">
-        <v>0</v>
-      </c>
-      <c r="G49" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1674,24 +1429,19 @@
       <c r="A50" t="n">
         <v>993</v>
       </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>1:41 PM</t>
-        </is>
+      <c r="B50" t="n">
+        <v>29775.52</v>
       </c>
       <c r="C50" t="n">
-        <v>29775.52</v>
+        <v>29805.52</v>
       </c>
       <c r="D50" t="n">
-        <v>29805.52</v>
+        <v>41.35</v>
       </c>
       <c r="E50" t="n">
-        <v>41.35</v>
+        <v>0</v>
       </c>
       <c r="F50" t="n">
-        <v>0</v>
-      </c>
-      <c r="G50" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1699,24 +1449,19 @@
       <c r="A51" t="n">
         <v>1002</v>
       </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>1:46 PM</t>
-        </is>
+      <c r="B51" t="n">
+        <v>30041.043333</v>
       </c>
       <c r="C51" t="n">
-        <v>30041.043333</v>
+        <v>30071.043333</v>
       </c>
       <c r="D51" t="n">
-        <v>30071.043333</v>
+        <v>13.076667</v>
       </c>
       <c r="E51" t="n">
-        <v>13.076667</v>
+        <v>0.336667</v>
       </c>
       <c r="F51" t="n">
-        <v>0.336667</v>
-      </c>
-      <c r="G51" t="n">
         <v>0.333333</v>
       </c>
     </row>
@@ -1724,24 +1469,19 @@
       <c r="A52" t="n">
         <v>1016</v>
       </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>1:53 PM</t>
-        </is>
+      <c r="B52" t="n">
+        <v>30454.73</v>
       </c>
       <c r="C52" t="n">
-        <v>30454.73</v>
+        <v>30484.73</v>
       </c>
       <c r="D52" t="n">
-        <v>30484.73</v>
+        <v>24.88</v>
       </c>
       <c r="E52" t="n">
-        <v>24.88</v>
+        <v>0</v>
       </c>
       <c r="F52" t="n">
-        <v>0</v>
-      </c>
-      <c r="G52" t="n">
         <v>2</v>
       </c>
     </row>
@@ -1749,24 +1489,19 @@
       <c r="A53" t="n">
         <v>1027</v>
       </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>1:59 PM</t>
-        </is>
+      <c r="B53" t="n">
+        <v>30807.17</v>
       </c>
       <c r="C53" t="n">
-        <v>30807.17</v>
+        <v>30837.17</v>
       </c>
       <c r="D53" t="n">
-        <v>30837.17</v>
+        <v>20.12</v>
       </c>
       <c r="E53" t="n">
-        <v>20.12</v>
+        <v>0</v>
       </c>
       <c r="F53" t="n">
-        <v>0</v>
-      </c>
-      <c r="G53" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1774,24 +1509,19 @@
       <c r="A54" t="n">
         <v>1036</v>
       </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>2:03 PM</t>
-        </is>
+      <c r="B54" t="n">
+        <v>31058.49</v>
       </c>
       <c r="C54" t="n">
-        <v>31058.49</v>
+        <v>31088.49</v>
       </c>
       <c r="D54" t="n">
-        <v>31088.49</v>
+        <v>60.24</v>
       </c>
       <c r="E54" t="n">
-        <v>60.24</v>
+        <v>0</v>
       </c>
       <c r="F54" t="n">
-        <v>0</v>
-      </c>
-      <c r="G54" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1799,24 +1529,19 @@
       <c r="A55" t="n">
         <v>1051</v>
       </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>2:10 PM</t>
-        </is>
+      <c r="B55" t="n">
+        <v>31511.296667</v>
       </c>
       <c r="C55" t="n">
-        <v>31511.296667</v>
+        <v>31541.296667</v>
       </c>
       <c r="D55" t="n">
-        <v>31541.296667</v>
+        <v>7.176667</v>
       </c>
       <c r="E55" t="n">
-        <v>7.176667</v>
+        <v>0</v>
       </c>
       <c r="F55" t="n">
-        <v>0</v>
-      </c>
-      <c r="G55" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1824,24 +1549,19 @@
       <c r="A56" t="n">
         <v>1066</v>
       </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>2:18 PM</t>
-        </is>
+      <c r="B56" t="n">
+        <v>31970.67</v>
       </c>
       <c r="C56" t="n">
-        <v>31970.67</v>
+        <v>32000.67</v>
       </c>
       <c r="D56" t="n">
-        <v>32000.67</v>
+        <v>17.12</v>
       </c>
       <c r="E56" t="n">
-        <v>17.12</v>
+        <v>0</v>
       </c>
       <c r="F56" t="n">
-        <v>0</v>
-      </c>
-      <c r="G56" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1849,24 +1569,19 @@
       <c r="A57" t="n">
         <v>1078</v>
       </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>2:24 PM</t>
-        </is>
+      <c r="B57" t="n">
+        <v>32329.13</v>
       </c>
       <c r="C57" t="n">
-        <v>32329.13</v>
+        <v>32359.13</v>
       </c>
       <c r="D57" t="n">
-        <v>32359.13</v>
+        <v>18.55</v>
       </c>
       <c r="E57" t="n">
-        <v>18.55</v>
+        <v>0</v>
       </c>
       <c r="F57" t="n">
-        <v>0</v>
-      </c>
-      <c r="G57" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1874,24 +1589,19 @@
       <c r="A58" t="n">
         <v>1086</v>
       </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>2:28 PM</t>
-        </is>
+      <c r="B58" t="n">
+        <v>32575.77</v>
       </c>
       <c r="C58" t="n">
-        <v>32575.77</v>
+        <v>32605.77</v>
       </c>
       <c r="D58" t="n">
-        <v>32605.77</v>
+        <v>21.33</v>
       </c>
       <c r="E58" t="n">
-        <v>21.33</v>
+        <v>0</v>
       </c>
       <c r="F58" t="n">
-        <v>0</v>
-      </c>
-      <c r="G58" t="n">
         <v>2</v>
       </c>
     </row>
@@ -1899,24 +1609,19 @@
       <c r="A59" t="n">
         <v>1103</v>
       </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>2:36 PM</t>
-        </is>
+      <c r="B59" t="n">
+        <v>33070.88</v>
       </c>
       <c r="C59" t="n">
-        <v>33070.88</v>
+        <v>33100.88</v>
       </c>
       <c r="D59" t="n">
-        <v>33100.88</v>
+        <v>25.1</v>
       </c>
       <c r="E59" t="n">
-        <v>25.1</v>
+        <v>0</v>
       </c>
       <c r="F59" t="n">
-        <v>0</v>
-      </c>
-      <c r="G59" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1924,24 +1629,19 @@
       <c r="A60" t="n">
         <v>1112</v>
       </c>
-      <c r="B60" t="inlineStr">
-        <is>
-          <t>2:41 PM</t>
-        </is>
+      <c r="B60" t="n">
+        <v>33353.96</v>
       </c>
       <c r="C60" t="n">
-        <v>33353.96</v>
+        <v>33383.96</v>
       </c>
       <c r="D60" t="n">
-        <v>33383.96</v>
+        <v>8.255000000000001</v>
       </c>
       <c r="E60" t="n">
-        <v>8.255000000000001</v>
+        <v>0</v>
       </c>
       <c r="F60" t="n">
-        <v>0</v>
-      </c>
-      <c r="G60" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -1949,24 +1649,19 @@
       <c r="A61" t="n">
         <v>1141</v>
       </c>
-      <c r="B61" t="inlineStr">
-        <is>
-          <t>2:55 PM</t>
-        </is>
+      <c r="B61" t="n">
+        <v>34219.87</v>
       </c>
       <c r="C61" t="n">
-        <v>34219.87</v>
+        <v>34249.87</v>
       </c>
       <c r="D61" t="n">
-        <v>34249.87</v>
+        <v>21.48</v>
       </c>
       <c r="E61" t="n">
-        <v>21.48</v>
+        <v>0</v>
       </c>
       <c r="F61" t="n">
-        <v>0</v>
-      </c>
-      <c r="G61" t="n">
         <v>2</v>
       </c>
     </row>
@@ -1974,24 +1669,19 @@
       <c r="A62" t="n">
         <v>1159</v>
       </c>
-      <c r="B62" t="inlineStr">
-        <is>
-          <t>3:04 PM</t>
-        </is>
+      <c r="B62" t="n">
+        <v>34751.028</v>
       </c>
       <c r="C62" t="n">
-        <v>34751.028</v>
+        <v>34781.028</v>
       </c>
       <c r="D62" t="n">
-        <v>34781.028</v>
+        <v>4.102</v>
       </c>
       <c r="E62" t="n">
-        <v>4.102</v>
+        <v>0</v>
       </c>
       <c r="F62" t="n">
-        <v>0</v>
-      </c>
-      <c r="G62" t="n">
         <v>0.2</v>
       </c>
     </row>
@@ -1999,24 +1689,19 @@
       <c r="A63" t="n">
         <v>1175</v>
       </c>
-      <c r="B63" t="inlineStr">
-        <is>
-          <t>3:12 PM</t>
-        </is>
+      <c r="B63" t="n">
+        <v>35229.795</v>
       </c>
       <c r="C63" t="n">
-        <v>35229.795</v>
+        <v>35259.795</v>
       </c>
       <c r="D63" t="n">
-        <v>35259.795</v>
+        <v>16.125</v>
       </c>
       <c r="E63" t="n">
-        <v>16.125</v>
+        <v>0</v>
       </c>
       <c r="F63" t="n">
-        <v>0</v>
-      </c>
-      <c r="G63" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -2024,24 +1709,19 @@
       <c r="A64" t="n">
         <v>1185</v>
       </c>
-      <c r="B64" t="inlineStr">
-        <is>
-          <t>3:17 PM</t>
-        </is>
+      <c r="B64" t="n">
+        <v>35530.52</v>
       </c>
       <c r="C64" t="n">
-        <v>35530.52</v>
+        <v>35560.52</v>
       </c>
       <c r="D64" t="n">
-        <v>35560.52</v>
+        <v>115.925</v>
       </c>
       <c r="E64" t="n">
-        <v>115.925</v>
+        <v>0</v>
       </c>
       <c r="F64" t="n">
-        <v>0</v>
-      </c>
-      <c r="G64" t="n">
         <v>3</v>
       </c>
     </row>
@@ -2049,24 +1729,19 @@
       <c r="A65" t="n">
         <v>1196</v>
       </c>
-      <c r="B65" t="inlineStr">
-        <is>
-          <t>3:23 PM</t>
-        </is>
+      <c r="B65" t="n">
+        <v>35858.715</v>
       </c>
       <c r="C65" t="n">
-        <v>35858.715</v>
+        <v>35888.715</v>
       </c>
       <c r="D65" t="n">
-        <v>35888.715</v>
+        <v>56.205</v>
       </c>
       <c r="E65" t="n">
-        <v>56.205</v>
+        <v>0</v>
       </c>
       <c r="F65" t="n">
-        <v>0</v>
-      </c>
-      <c r="G65" t="n">
         <v>2</v>
       </c>
     </row>
@@ -2074,24 +1749,19 @@
       <c r="A66" t="n">
         <v>1204</v>
       </c>
-      <c r="B66" t="inlineStr">
-        <is>
-          <t>3:27 PM</t>
-        </is>
+      <c r="B66" t="n">
+        <v>36097.916667</v>
       </c>
       <c r="C66" t="n">
-        <v>36097.916667</v>
+        <v>36127.916667</v>
       </c>
       <c r="D66" t="n">
-        <v>36127.916667</v>
+        <v>82.06</v>
       </c>
       <c r="E66" t="n">
-        <v>82.06</v>
+        <v>0</v>
       </c>
       <c r="F66" t="n">
-        <v>0</v>
-      </c>
-      <c r="G66" t="n">
         <v>1.333333</v>
       </c>
     </row>
@@ -2099,24 +1769,19 @@
       <c r="A67" t="n">
         <v>1214</v>
       </c>
-      <c r="B67" t="inlineStr">
-        <is>
-          <t>3:32 PM</t>
-        </is>
+      <c r="B67" t="n">
+        <v>36391.61</v>
       </c>
       <c r="C67" t="n">
-        <v>36391.61</v>
+        <v>36421.61</v>
       </c>
       <c r="D67" t="n">
-        <v>36421.61</v>
+        <v>96.52</v>
       </c>
       <c r="E67" t="n">
-        <v>96.52</v>
+        <v>0</v>
       </c>
       <c r="F67" t="n">
-        <v>0</v>
-      </c>
-      <c r="G67" t="n">
         <v>7</v>
       </c>
     </row>
@@ -2124,24 +1789,19 @@
       <c r="A68" t="n">
         <v>1221</v>
       </c>
-      <c r="B68" t="inlineStr">
-        <is>
-          <t>3:35 PM</t>
-        </is>
+      <c r="B68" t="n">
+        <v>36616.4</v>
       </c>
       <c r="C68" t="n">
-        <v>36616.4</v>
+        <v>36646.4</v>
       </c>
       <c r="D68" t="n">
-        <v>36646.4</v>
+        <v>23.47</v>
       </c>
       <c r="E68" t="n">
-        <v>23.47</v>
+        <v>0</v>
       </c>
       <c r="F68" t="n">
-        <v>0</v>
-      </c>
-      <c r="G68" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2149,24 +1809,19 @@
       <c r="A69" t="n">
         <v>1233</v>
       </c>
-      <c r="B69" t="inlineStr">
-        <is>
-          <t>3:41 PM</t>
-        </is>
+      <c r="B69" t="n">
+        <v>36983.29</v>
       </c>
       <c r="C69" t="n">
-        <v>36983.29</v>
+        <v>37013.29</v>
       </c>
       <c r="D69" t="n">
-        <v>37013.29</v>
+        <v>12.33</v>
       </c>
       <c r="E69" t="n">
-        <v>12.33</v>
+        <v>0</v>
       </c>
       <c r="F69" t="n">
-        <v>0</v>
-      </c>
-      <c r="G69" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2174,24 +1829,19 @@
       <c r="A70" t="n">
         <v>1245</v>
       </c>
-      <c r="B70" t="inlineStr">
-        <is>
-          <t>3:47 PM</t>
-        </is>
+      <c r="B70" t="n">
+        <v>37332.09</v>
       </c>
       <c r="C70" t="n">
-        <v>37332.09</v>
+        <v>37362.09</v>
       </c>
       <c r="D70" t="n">
-        <v>37362.09</v>
+        <v>193.12</v>
       </c>
       <c r="E70" t="n">
-        <v>193.12</v>
+        <v>0</v>
       </c>
       <c r="F70" t="n">
-        <v>0</v>
-      </c>
-      <c r="G70" t="n">
         <v>6</v>
       </c>
     </row>
@@ -2199,24 +1849,19 @@
       <c r="A71" t="n">
         <v>1257</v>
       </c>
-      <c r="B71" t="inlineStr">
-        <is>
-          <t>3:53 PM</t>
-        </is>
+      <c r="B71" t="n">
+        <v>37684.8</v>
       </c>
       <c r="C71" t="n">
-        <v>37684.8</v>
+        <v>37714.8</v>
       </c>
       <c r="D71" t="n">
-        <v>37714.8</v>
+        <v>36.82</v>
       </c>
       <c r="E71" t="n">
-        <v>36.82</v>
+        <v>0</v>
       </c>
       <c r="F71" t="n">
-        <v>0</v>
-      </c>
-      <c r="G71" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2224,24 +1869,19 @@
       <c r="A72" t="n">
         <v>1264</v>
       </c>
-      <c r="B72" t="inlineStr">
-        <is>
-          <t>3:57 PM</t>
-        </is>
+      <c r="B72" t="n">
+        <v>37898.075</v>
       </c>
       <c r="C72" t="n">
-        <v>37898.075</v>
+        <v>37928.075</v>
       </c>
       <c r="D72" t="n">
-        <v>37928.075</v>
+        <v>18.055</v>
       </c>
       <c r="E72" t="n">
-        <v>18.055</v>
+        <v>0</v>
       </c>
       <c r="F72" t="n">
-        <v>0</v>
-      </c>
-      <c r="G72" t="n">
         <v>0.25</v>
       </c>
     </row>
@@ -2249,24 +1889,19 @@
       <c r="A73" t="n">
         <v>1273</v>
       </c>
-      <c r="B73" t="inlineStr">
-        <is>
-          <t>4:02 PM</t>
-        </is>
+      <c r="B73" t="n">
+        <v>38186.04</v>
       </c>
       <c r="C73" t="n">
-        <v>38186.04</v>
+        <v>38216.04</v>
       </c>
       <c r="D73" t="n">
-        <v>38216.04</v>
+        <v>28.77</v>
       </c>
       <c r="E73" t="n">
-        <v>28.77</v>
+        <v>0</v>
       </c>
       <c r="F73" t="n">
-        <v>0</v>
-      </c>
-      <c r="G73" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2274,24 +1909,19 @@
       <c r="A74" t="n">
         <v>1283</v>
       </c>
-      <c r="B74" t="inlineStr">
-        <is>
-          <t>4:06 PM</t>
-        </is>
+      <c r="B74" t="n">
+        <v>38479.19</v>
       </c>
       <c r="C74" t="n">
-        <v>38479.19</v>
+        <v>38509.19</v>
       </c>
       <c r="D74" t="n">
-        <v>38509.19</v>
+        <v>51.24</v>
       </c>
       <c r="E74" t="n">
-        <v>51.24</v>
+        <v>0</v>
       </c>
       <c r="F74" t="n">
-        <v>0</v>
-      </c>
-      <c r="G74" t="n">
         <v>3</v>
       </c>
     </row>
@@ -2299,24 +1929,19 @@
       <c r="A75" t="n">
         <v>1291</v>
       </c>
-      <c r="B75" t="inlineStr">
-        <is>
-          <t>4:11 PM</t>
-        </is>
+      <c r="B75" t="n">
+        <v>38728.38</v>
       </c>
       <c r="C75" t="n">
-        <v>38728.38</v>
+        <v>38758.38</v>
       </c>
       <c r="D75" t="n">
-        <v>38758.38</v>
+        <v>100.57</v>
       </c>
       <c r="E75" t="n">
-        <v>100.57</v>
+        <v>0</v>
       </c>
       <c r="F75" t="n">
-        <v>0</v>
-      </c>
-      <c r="G75" t="n">
         <v>2</v>
       </c>
     </row>
@@ -2324,24 +1949,19 @@
       <c r="A76" t="n">
         <v>1302</v>
       </c>
-      <c r="B76" t="inlineStr">
-        <is>
-          <t>4:16 PM</t>
-        </is>
+      <c r="B76" t="n">
+        <v>39032.49</v>
       </c>
       <c r="C76" t="n">
-        <v>39032.49</v>
+        <v>39062.49</v>
       </c>
       <c r="D76" t="n">
-        <v>39062.49</v>
+        <v>230.5</v>
       </c>
       <c r="E76" t="n">
-        <v>230.5</v>
+        <v>0</v>
       </c>
       <c r="F76" t="n">
-        <v>0</v>
-      </c>
-      <c r="G76" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2349,24 +1969,19 @@
       <c r="A77" t="n">
         <v>1311</v>
       </c>
-      <c r="B77" t="inlineStr">
-        <is>
-          <t>4:20 PM</t>
-        </is>
+      <c r="B77" t="n">
+        <v>39315.5</v>
       </c>
       <c r="C77" t="n">
-        <v>39315.5</v>
+        <v>39345.5</v>
       </c>
       <c r="D77" t="n">
-        <v>39345.5</v>
+        <v>76.02</v>
       </c>
       <c r="E77" t="n">
-        <v>76.02</v>
+        <v>0</v>
       </c>
       <c r="F77" t="n">
-        <v>0</v>
-      </c>
-      <c r="G77" t="n">
         <v>1.5</v>
       </c>
     </row>
@@ -2374,24 +1989,19 @@
       <c r="A78" t="n">
         <v>1318</v>
       </c>
-      <c r="B78" t="inlineStr">
-        <is>
-          <t>4:24 PM</t>
-        </is>
+      <c r="B78" t="n">
+        <v>39526.18</v>
       </c>
       <c r="C78" t="n">
-        <v>39526.18</v>
+        <v>39556.18</v>
       </c>
       <c r="D78" t="n">
-        <v>39556.18</v>
+        <v>111.31</v>
       </c>
       <c r="E78" t="n">
-        <v>111.31</v>
+        <v>0</v>
       </c>
       <c r="F78" t="n">
-        <v>0</v>
-      </c>
-      <c r="G78" t="n">
         <v>2.5</v>
       </c>
     </row>
@@ -2399,24 +2009,19 @@
       <c r="A79" t="n">
         <v>1326</v>
       </c>
-      <c r="B79" t="inlineStr">
-        <is>
-          <t>4:28 PM</t>
-        </is>
+      <c r="B79" t="n">
+        <v>39760.395</v>
       </c>
       <c r="C79" t="n">
-        <v>39760.395</v>
+        <v>39790.395</v>
       </c>
       <c r="D79" t="n">
-        <v>39790.395</v>
+        <v>17.51</v>
       </c>
       <c r="E79" t="n">
-        <v>17.51</v>
+        <v>0</v>
       </c>
       <c r="F79" t="n">
-        <v>0</v>
-      </c>
-      <c r="G79" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2424,24 +2029,19 @@
       <c r="A80" t="n">
         <v>1335</v>
       </c>
-      <c r="B80" t="inlineStr">
-        <is>
-          <t>4:32 PM</t>
-        </is>
+      <c r="B80" t="n">
+        <v>40027.72</v>
       </c>
       <c r="C80" t="n">
-        <v>40027.72</v>
+        <v>40057.72</v>
       </c>
       <c r="D80" t="n">
-        <v>40057.72</v>
+        <v>47.705</v>
       </c>
       <c r="E80" t="n">
-        <v>47.705</v>
+        <v>0</v>
       </c>
       <c r="F80" t="n">
-        <v>0</v>
-      </c>
-      <c r="G80" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -2449,24 +2049,19 @@
       <c r="A81" t="n">
         <v>1345</v>
       </c>
-      <c r="B81" t="inlineStr">
-        <is>
-          <t>4:38 PM</t>
-        </is>
+      <c r="B81" t="n">
+        <v>40347.76</v>
       </c>
       <c r="C81" t="n">
-        <v>40347.76</v>
+        <v>40377.76</v>
       </c>
       <c r="D81" t="n">
-        <v>40377.76</v>
+        <v>94.73999999999999</v>
       </c>
       <c r="E81" t="n">
-        <v>94.73999999999999</v>
+        <v>0</v>
       </c>
       <c r="F81" t="n">
-        <v>0</v>
-      </c>
-      <c r="G81" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2474,24 +2069,19 @@
       <c r="A82" t="n">
         <v>1357</v>
       </c>
-      <c r="B82" t="inlineStr">
-        <is>
-          <t>4:43 PM</t>
-        </is>
+      <c r="B82" t="n">
+        <v>40690.25</v>
       </c>
       <c r="C82" t="n">
-        <v>40690.25</v>
+        <v>40720.25</v>
       </c>
       <c r="D82" t="n">
-        <v>40720.25</v>
+        <v>163.16</v>
       </c>
       <c r="E82" t="n">
-        <v>163.16</v>
+        <v>0</v>
       </c>
       <c r="F82" t="n">
-        <v>0</v>
-      </c>
-      <c r="G82" t="n">
         <v>5</v>
       </c>
     </row>
@@ -2499,24 +2089,19 @@
       <c r="A83" t="n">
         <v>1372</v>
       </c>
-      <c r="B83" t="inlineStr">
-        <is>
-          <t>4:51 PM</t>
-        </is>
+      <c r="B83" t="n">
+        <v>41141.465</v>
       </c>
       <c r="C83" t="n">
-        <v>41141.465</v>
+        <v>41171.465</v>
       </c>
       <c r="D83" t="n">
-        <v>41171.465</v>
+        <v>98.08</v>
       </c>
       <c r="E83" t="n">
-        <v>98.08</v>
+        <v>0</v>
       </c>
       <c r="F83" t="n">
-        <v>0</v>
-      </c>
-      <c r="G83" t="n">
         <v>5</v>
       </c>
     </row>
@@ -2524,24 +2109,19 @@
       <c r="A84" t="n">
         <v>1382</v>
       </c>
-      <c r="B84" t="inlineStr">
-        <is>
-          <t>4:56 PM</t>
-        </is>
+      <c r="B84" t="n">
+        <v>41437.05</v>
       </c>
       <c r="C84" t="n">
-        <v>41437.05</v>
+        <v>41467.05</v>
       </c>
       <c r="D84" t="n">
-        <v>41467.05</v>
+        <v>13.86</v>
       </c>
       <c r="E84" t="n">
-        <v>13.86</v>
+        <v>0</v>
       </c>
       <c r="F84" t="n">
-        <v>0</v>
-      </c>
-      <c r="G84" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -2549,24 +2129,19 @@
       <c r="A85" t="n">
         <v>1391</v>
       </c>
-      <c r="B85" t="inlineStr">
-        <is>
-          <t>5:01 PM</t>
-        </is>
+      <c r="B85" t="n">
+        <v>41726.28</v>
       </c>
       <c r="C85" t="n">
-        <v>41726.28</v>
+        <v>41756.28</v>
       </c>
       <c r="D85" t="n">
-        <v>41756.28</v>
+        <v>40.32</v>
       </c>
       <c r="E85" t="n">
-        <v>40.32</v>
+        <v>0</v>
       </c>
       <c r="F85" t="n">
-        <v>0</v>
-      </c>
-      <c r="G85" t="n">
         <v>2</v>
       </c>
     </row>
@@ -2574,24 +2149,19 @@
       <c r="A86" t="n">
         <v>1404</v>
       </c>
-      <c r="B86" t="inlineStr">
-        <is>
-          <t>5:07 PM</t>
-        </is>
+      <c r="B86" t="n">
+        <v>42097.02</v>
       </c>
       <c r="C86" t="n">
-        <v>42097.02</v>
+        <v>42127.02</v>
       </c>
       <c r="D86" t="n">
-        <v>42127.02</v>
+        <v>13.55</v>
       </c>
       <c r="E86" t="n">
-        <v>13.55</v>
+        <v>0</v>
       </c>
       <c r="F86" t="n">
-        <v>0</v>
-      </c>
-      <c r="G86" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2599,24 +2169,19 @@
       <c r="A87" t="n">
         <v>1412</v>
       </c>
-      <c r="B87" t="inlineStr">
-        <is>
-          <t>5:11 PM</t>
-        </is>
+      <c r="B87" t="n">
+        <v>42334.07</v>
       </c>
       <c r="C87" t="n">
-        <v>42334.07</v>
+        <v>42364.07</v>
       </c>
       <c r="D87" t="n">
-        <v>42364.07</v>
+        <v>101.66</v>
       </c>
       <c r="E87" t="n">
-        <v>101.66</v>
+        <v>0</v>
       </c>
       <c r="F87" t="n">
-        <v>0</v>
-      </c>
-      <c r="G87" t="n">
         <v>2</v>
       </c>
     </row>
@@ -2624,24 +2189,19 @@
       <c r="A88" t="n">
         <v>1419</v>
       </c>
-      <c r="B88" t="inlineStr">
-        <is>
-          <t>5:15 PM</t>
-        </is>
+      <c r="B88" t="n">
+        <v>42568.78</v>
       </c>
       <c r="C88" t="n">
-        <v>42568.78</v>
+        <v>42598.78</v>
       </c>
       <c r="D88" t="n">
-        <v>42598.78</v>
+        <v>8.369999999999999</v>
       </c>
       <c r="E88" t="n">
-        <v>8.369999999999999</v>
+        <v>0</v>
       </c>
       <c r="F88" t="n">
-        <v>0</v>
-      </c>
-      <c r="G88" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2649,24 +2209,19 @@
       <c r="A89" t="n">
         <v>1427</v>
       </c>
-      <c r="B89" t="inlineStr">
-        <is>
-          <t>5:19 PM</t>
-        </is>
+      <c r="B89" t="n">
+        <v>42809.97</v>
       </c>
       <c r="C89" t="n">
-        <v>42809.97</v>
+        <v>42839.97</v>
       </c>
       <c r="D89" t="n">
-        <v>42839.97</v>
+        <v>161.82</v>
       </c>
       <c r="E89" t="n">
-        <v>161.82</v>
+        <v>0</v>
       </c>
       <c r="F89" t="n">
-        <v>0</v>
-      </c>
-      <c r="G89" t="n">
         <v>9</v>
       </c>
     </row>
@@ -2674,24 +2229,19 @@
       <c r="A90" t="n">
         <v>1441</v>
       </c>
-      <c r="B90" t="inlineStr">
-        <is>
-          <t>5:26 PM</t>
-        </is>
+      <c r="B90" t="n">
+        <v>43229.93</v>
       </c>
       <c r="C90" t="n">
-        <v>43229.93</v>
+        <v>43259.93</v>
       </c>
       <c r="D90" t="n">
-        <v>43259.93</v>
+        <v>24.11</v>
       </c>
       <c r="E90" t="n">
-        <v>24.11</v>
+        <v>0</v>
       </c>
       <c r="F90" t="n">
-        <v>0</v>
-      </c>
-      <c r="G90" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2699,24 +2249,19 @@
       <c r="A91" t="n">
         <v>1451</v>
       </c>
-      <c r="B91" t="inlineStr">
-        <is>
-          <t>5:30 PM</t>
-        </is>
+      <c r="B91" t="n">
+        <v>43516.02</v>
       </c>
       <c r="C91" t="n">
-        <v>43516.02</v>
+        <v>43546.02</v>
       </c>
       <c r="D91" t="n">
-        <v>43546.02</v>
+        <v>88.58</v>
       </c>
       <c r="E91" t="n">
-        <v>88.58</v>
+        <v>0</v>
       </c>
       <c r="F91" t="n">
-        <v>0</v>
-      </c>
-      <c r="G91" t="n">
         <v>2</v>
       </c>
     </row>
@@ -2724,24 +2269,19 @@
       <c r="A92" t="n">
         <v>1459</v>
       </c>
-      <c r="B92" t="inlineStr">
-        <is>
-          <t>5:34 PM</t>
-        </is>
+      <c r="B92" t="n">
+        <v>43757.37</v>
       </c>
       <c r="C92" t="n">
-        <v>43757.37</v>
+        <v>43787.37</v>
       </c>
       <c r="D92" t="n">
-        <v>43787.37</v>
+        <v>15.4</v>
       </c>
       <c r="E92" t="n">
-        <v>15.4</v>
+        <v>0</v>
       </c>
       <c r="F92" t="n">
-        <v>0</v>
-      </c>
-      <c r="G92" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -2749,24 +2289,19 @@
       <c r="A93" t="n">
         <v>1471</v>
       </c>
-      <c r="B93" t="inlineStr">
-        <is>
-          <t>5:41 PM</t>
-        </is>
+      <c r="B93" t="n">
+        <v>44128.76</v>
       </c>
       <c r="C93" t="n">
-        <v>44128.76</v>
+        <v>44158.76</v>
       </c>
       <c r="D93" t="n">
-        <v>44158.76</v>
+        <v>5.15</v>
       </c>
       <c r="E93" t="n">
-        <v>5.15</v>
+        <v>0</v>
       </c>
       <c r="F93" t="n">
-        <v>0</v>
-      </c>
-      <c r="G93" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2774,24 +2309,19 @@
       <c r="A94" t="n">
         <v>1479</v>
       </c>
-      <c r="B94" t="inlineStr">
-        <is>
-          <t>5:44 PM</t>
-        </is>
+      <c r="B94" t="n">
+        <v>44340.68</v>
       </c>
       <c r="C94" t="n">
-        <v>44340.68</v>
+        <v>44370.68</v>
       </c>
       <c r="D94" t="n">
-        <v>44370.68</v>
+        <v>49.65</v>
       </c>
       <c r="E94" t="n">
-        <v>49.65</v>
+        <v>0</v>
       </c>
       <c r="F94" t="n">
-        <v>0</v>
-      </c>
-      <c r="G94" t="n">
         <v>3</v>
       </c>
     </row>
@@ -2799,24 +2329,19 @@
       <c r="A95" t="n">
         <v>1492</v>
       </c>
-      <c r="B95" t="inlineStr">
-        <is>
-          <t>5:51 PM</t>
-        </is>
+      <c r="B95" t="n">
+        <v>44738.87</v>
       </c>
       <c r="C95" t="n">
-        <v>44738.87</v>
+        <v>44768.87</v>
       </c>
       <c r="D95" t="n">
-        <v>44768.87</v>
+        <v>22.62</v>
       </c>
       <c r="E95" t="n">
-        <v>22.62</v>
+        <v>0</v>
       </c>
       <c r="F95" t="n">
-        <v>0</v>
-      </c>
-      <c r="G95" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2824,24 +2349,19 @@
       <c r="A96" t="n">
         <v>1500</v>
       </c>
-      <c r="B96" t="inlineStr">
-        <is>
-          <t>5:55 PM</t>
-        </is>
+      <c r="B96" t="n">
+        <v>44976.08</v>
       </c>
       <c r="C96" t="n">
-        <v>44976.08</v>
+        <v>45006.08</v>
       </c>
       <c r="D96" t="n">
-        <v>45006.08</v>
+        <v>17.24</v>
       </c>
       <c r="E96" t="n">
-        <v>17.24</v>
+        <v>0</v>
       </c>
       <c r="F96" t="n">
-        <v>0</v>
-      </c>
-      <c r="G96" t="n">
         <v>2</v>
       </c>
     </row>
@@ -2849,24 +2369,19 @@
       <c r="A97" t="n">
         <v>1510</v>
       </c>
-      <c r="B97" t="inlineStr">
-        <is>
-          <t>6:00 PM</t>
-        </is>
+      <c r="B97" t="n">
+        <v>45289.285</v>
       </c>
       <c r="C97" t="n">
-        <v>45289.285</v>
+        <v>45319.285</v>
       </c>
       <c r="D97" t="n">
-        <v>45319.285</v>
+        <v>12.07</v>
       </c>
       <c r="E97" t="n">
-        <v>12.07</v>
+        <v>0</v>
       </c>
       <c r="F97" t="n">
-        <v>0</v>
-      </c>
-      <c r="G97" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2874,24 +2389,19 @@
       <c r="A98" t="n">
         <v>1522</v>
       </c>
-      <c r="B98" t="inlineStr">
-        <is>
-          <t>6:06 PM</t>
-        </is>
+      <c r="B98" t="n">
+        <v>45637.495</v>
       </c>
       <c r="C98" t="n">
-        <v>45637.495</v>
+        <v>45667.495</v>
       </c>
       <c r="D98" t="n">
-        <v>45667.495</v>
+        <v>33.28</v>
       </c>
       <c r="E98" t="n">
-        <v>33.28</v>
+        <v>0</v>
       </c>
       <c r="F98" t="n">
-        <v>0</v>
-      </c>
-      <c r="G98" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -2899,24 +2409,19 @@
       <c r="A99" t="n">
         <v>1535</v>
       </c>
-      <c r="B99" t="inlineStr">
-        <is>
-          <t>6:12 PM</t>
-        </is>
+      <c r="B99" t="n">
+        <v>46024.31</v>
       </c>
       <c r="C99" t="n">
-        <v>46024.31</v>
+        <v>46054.31</v>
       </c>
       <c r="D99" t="n">
-        <v>46054.31</v>
+        <v>7.985</v>
       </c>
       <c r="E99" t="n">
-        <v>7.985</v>
+        <v>0</v>
       </c>
       <c r="F99" t="n">
-        <v>0</v>
-      </c>
-      <c r="G99" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2924,24 +2429,19 @@
       <c r="A100" t="n">
         <v>1551</v>
       </c>
-      <c r="B100" t="inlineStr">
-        <is>
-          <t>6:20 PM</t>
-        </is>
+      <c r="B100" t="n">
+        <v>46502.28</v>
       </c>
       <c r="C100" t="n">
-        <v>46502.28</v>
+        <v>46532.28</v>
       </c>
       <c r="D100" t="n">
-        <v>46532.28</v>
+        <v>39.27</v>
       </c>
       <c r="E100" t="n">
-        <v>39.27</v>
+        <v>1.01</v>
       </c>
       <c r="F100" t="n">
-        <v>1.01</v>
-      </c>
-      <c r="G100" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2949,24 +2449,19 @@
       <c r="A101" t="n">
         <v>1611</v>
       </c>
-      <c r="B101" t="inlineStr">
-        <is>
-          <t>6:50 PM</t>
-        </is>
+      <c r="B101" t="n">
+        <v>48310.16</v>
       </c>
       <c r="C101" t="n">
-        <v>48310.16</v>
+        <v>48340.16</v>
       </c>
       <c r="D101" t="n">
-        <v>48340.16</v>
+        <v>3.305</v>
       </c>
       <c r="E101" t="n">
-        <v>3.305</v>
+        <v>0</v>
       </c>
       <c r="F101" t="n">
-        <v>0</v>
-      </c>
-      <c r="G101" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>